<commit_message>
Bugfix/Update wrong column names
</commit_message>
<xml_diff>
--- a/reports/approved_requests/templates/xlsx/template.xlsx
+++ b/reports/approved_requests/templates/xlsx/template.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">End_Customer_External_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Provider _ID</t>
+    <t xml:space="preserve">Provider__ID</t>
   </si>
   <si>
     <t xml:space="preserve">Provider_Name</t>
@@ -318,11 +318,11 @@
   </sheetPr>
   <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
@@ -358,7 +358,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="35" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="35" style="1" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Bugfix/Update wrong column names (#2)
</commit_message>
<xml_diff>
--- a/reports/approved_requests/templates/xlsx/template.xlsx
+++ b/reports/approved_requests/templates/xlsx/template.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">End_Customer_External_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Provider _ID</t>
+    <t xml:space="preserve">Provider__ID</t>
   </si>
   <si>
     <t xml:space="preserve">Provider_Name</t>
@@ -318,11 +318,11 @@
   </sheetPr>
   <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
@@ -358,7 +358,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="35" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="35" style="1" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>